<commit_message>
AMU and GA minor code changes
</commit_message>
<xml_diff>
--- a/Antimicrobial Use workspace/Data/Raw/AMU_ euros per ton.xlsx
+++ b/Antimicrobial Use workspace/Data/Raw/AMU_ euros per ton.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbmart\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E9470FDF-0550-4408-B2EB-B8B5D04BBD30}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4A7AA3-0646-4D86-94DE-C949B4F8E1DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{42967861-71FB-4F7B-8C72-E6FCF00D85D6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>* Overall sales, in tonnes of active substance, in 2020, total for 31 countries</t>
   </si>
@@ -61,13 +61,37 @@
   </si>
   <si>
     <t>Volume sales 2020 (euros)**</t>
+  </si>
+  <si>
+    <t>Upper limit</t>
+  </si>
+  <si>
+    <t>Reference price Europe</t>
+  </si>
+  <si>
+    <t>* African markets</t>
+  </si>
+  <si>
+    <t>** ME and SEA markets</t>
+  </si>
+  <si>
+    <t>Reference price: Europe data above</t>
+  </si>
+  <si>
+    <t>Upper variation of price:  22% to 42%*</t>
+  </si>
+  <si>
+    <t>Lower  variation of price: 15 to 25%**</t>
+  </si>
+  <si>
+    <t>Source: expert opinion, pending other expert insights</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,8 +150,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -139,8 +178,13 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -172,27 +216,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
@@ -204,8 +249,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -519,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47E5D133-92A0-49CD-A09A-97A9C868D634}">
-  <dimension ref="A3:E11"/>
+  <dimension ref="A3:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -534,118 +594,171 @@
     <col min="5" max="5" width="11.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="7"/>
-      <c r="B3" s="12" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="4"/>
+      <c r="B3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="9" t="s">
+      <c r="G3" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="4">
         <v>32.6</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="3">
         <f>B4*C8/100</f>
         <v>2216800000</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="11" t="s">
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="7">
         <v>11.9</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="5">
         <f>B5*C8/100</f>
         <v>809200000</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="5">
         <f>5577.8</f>
         <v>5577.8</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="5">
         <f>C5/D5</f>
         <v>145075.11922263258</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="4">
         <v>28.7</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="3">
         <f>B6*C8/100</f>
         <v>1951600000</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="9" t="s">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="4">
         <v>26.8</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="3">
         <f>B7*C8/100</f>
         <v>1822400000</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="9" t="s">
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="4">
         <f>SUM(B4:B7)</f>
         <v>100</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="5">
         <v>6800000000</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:5" ht="43" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="5" t="s">
+      <c r="D8" s="4"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" ht="43" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="4" t="s">
+      <c r="C9" s="11"/>
+      <c r="D9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" ht="23" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="10"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="16"/>
+      <c r="C15" s="15"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="16"/>
+      <c r="C16" s="15"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -653,5 +766,6 @@
     <mergeCell ref="A10:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>